<commit_message>
filtered master svpr for new regs using the data of new_reg
</commit_message>
<xml_diff>
--- a/new_registrations_after_21DEC2023.xlsx
+++ b/new_registrations_after_21DEC2023.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\TO BE SENT TO VCI\FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\SVPR TO ELECROLL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="946">
   <si>
     <t>Dr. Gauranga Mahato</t>
   </si>
@@ -2251,6 +2251,621 @@
   </si>
   <si>
     <t>Name of State/U.T. Veterinary Council: ASSAM VETERINARY COUNCIL</t>
+  </si>
+  <si>
+    <t>only asm-id</t>
+  </si>
+  <si>
+    <t>ASM-0138</t>
+  </si>
+  <si>
+    <t>ASM-0149</t>
+  </si>
+  <si>
+    <t>ASM-0198</t>
+  </si>
+  <si>
+    <t>ASM-0211</t>
+  </si>
+  <si>
+    <t>ASM-0369</t>
+  </si>
+  <si>
+    <t>ASM-0404</t>
+  </si>
+  <si>
+    <t>ASM-0414</t>
+  </si>
+  <si>
+    <t>ASM-0425</t>
+  </si>
+  <si>
+    <t>ASM-0428</t>
+  </si>
+  <si>
+    <t>ASM-0429</t>
+  </si>
+  <si>
+    <t>ASM-0507</t>
+  </si>
+  <si>
+    <t>ASM-0522</t>
+  </si>
+  <si>
+    <t>ASM-0583</t>
+  </si>
+  <si>
+    <t>ASM-0664</t>
+  </si>
+  <si>
+    <t>ASM-0668</t>
+  </si>
+  <si>
+    <t>ASM-0669</t>
+  </si>
+  <si>
+    <t>ASM-0675</t>
+  </si>
+  <si>
+    <t>ASM-0679</t>
+  </si>
+  <si>
+    <t>ASM-0694</t>
+  </si>
+  <si>
+    <t>ASM-0696</t>
+  </si>
+  <si>
+    <t>ASM-0709</t>
+  </si>
+  <si>
+    <t>ASM-0746</t>
+  </si>
+  <si>
+    <t>ASM-0757</t>
+  </si>
+  <si>
+    <t>ASM-0819</t>
+  </si>
+  <si>
+    <t>ASM-0825</t>
+  </si>
+  <si>
+    <t>ASM-0829</t>
+  </si>
+  <si>
+    <t>ASM-0850</t>
+  </si>
+  <si>
+    <t>ASM-0873</t>
+  </si>
+  <si>
+    <t>ASM-0877</t>
+  </si>
+  <si>
+    <t>ASM-0882</t>
+  </si>
+  <si>
+    <t>ASM-0904</t>
+  </si>
+  <si>
+    <t>ASM-0918</t>
+  </si>
+  <si>
+    <t>ASM-0924</t>
+  </si>
+  <si>
+    <t>ASM-0925</t>
+  </si>
+  <si>
+    <t>ASM-0959</t>
+  </si>
+  <si>
+    <t>ASM-0962</t>
+  </si>
+  <si>
+    <t>ASM-0964</t>
+  </si>
+  <si>
+    <t>ASM-0992</t>
+  </si>
+  <si>
+    <t>ASM-1006</t>
+  </si>
+  <si>
+    <t>ASM-1024</t>
+  </si>
+  <si>
+    <t>ASM-1030</t>
+  </si>
+  <si>
+    <t>ASM-1082</t>
+  </si>
+  <si>
+    <t>ASM-1108</t>
+  </si>
+  <si>
+    <t>ASM-1113</t>
+  </si>
+  <si>
+    <t>ASM-1135</t>
+  </si>
+  <si>
+    <t>ASM-1148</t>
+  </si>
+  <si>
+    <t>ASM-1160</t>
+  </si>
+  <si>
+    <t>ASM-1183</t>
+  </si>
+  <si>
+    <t>ASM-1185</t>
+  </si>
+  <si>
+    <t>ASM-1214</t>
+  </si>
+  <si>
+    <t>ASM-1224</t>
+  </si>
+  <si>
+    <t>ASM-1232</t>
+  </si>
+  <si>
+    <t>ASM-1240</t>
+  </si>
+  <si>
+    <t>ASM-1269</t>
+  </si>
+  <si>
+    <t>ASM-1296</t>
+  </si>
+  <si>
+    <t>ASM-1321</t>
+  </si>
+  <si>
+    <t>ASM-1363</t>
+  </si>
+  <si>
+    <t>ASM-1375</t>
+  </si>
+  <si>
+    <t>ASM-1383</t>
+  </si>
+  <si>
+    <t>ASM-1398</t>
+  </si>
+  <si>
+    <t>ASM-1403</t>
+  </si>
+  <si>
+    <t>ASM-1421</t>
+  </si>
+  <si>
+    <t>ASM-1467</t>
+  </si>
+  <si>
+    <t>ASM-1473</t>
+  </si>
+  <si>
+    <t>ASM-1501</t>
+  </si>
+  <si>
+    <t>ASM-1522</t>
+  </si>
+  <si>
+    <t>ASM-1526</t>
+  </si>
+  <si>
+    <t>ASM-1535</t>
+  </si>
+  <si>
+    <t>ASM-1538</t>
+  </si>
+  <si>
+    <t>ASM-1540</t>
+  </si>
+  <si>
+    <t>ASM-1548</t>
+  </si>
+  <si>
+    <t>ASM-1572</t>
+  </si>
+  <si>
+    <t>ASM-1599</t>
+  </si>
+  <si>
+    <t>ASM-1602</t>
+  </si>
+  <si>
+    <t>ASM-1603</t>
+  </si>
+  <si>
+    <t>ASM-1604</t>
+  </si>
+  <si>
+    <t>ASM-1606</t>
+  </si>
+  <si>
+    <t>ASM-1631</t>
+  </si>
+  <si>
+    <t>ASM-1639</t>
+  </si>
+  <si>
+    <t>ASM-1648</t>
+  </si>
+  <si>
+    <t>ASM-1658</t>
+  </si>
+  <si>
+    <t>ASM-1666</t>
+  </si>
+  <si>
+    <t>ASM-1689</t>
+  </si>
+  <si>
+    <t>ASM-1707</t>
+  </si>
+  <si>
+    <t>ASM-1731</t>
+  </si>
+  <si>
+    <t>ASM-1732</t>
+  </si>
+  <si>
+    <t>ASM-1759</t>
+  </si>
+  <si>
+    <t>ASM-1768</t>
+  </si>
+  <si>
+    <t>ASM-1772</t>
+  </si>
+  <si>
+    <t>ASM-1775</t>
+  </si>
+  <si>
+    <t>ASM-1790</t>
+  </si>
+  <si>
+    <t>ASM-1860</t>
+  </si>
+  <si>
+    <t>ASM-1872</t>
+  </si>
+  <si>
+    <t>ASM-1906</t>
+  </si>
+  <si>
+    <t>ASM-1908</t>
+  </si>
+  <si>
+    <t>ASM-1916</t>
+  </si>
+  <si>
+    <t>ASM-1918</t>
+  </si>
+  <si>
+    <t>ASM-1927</t>
+  </si>
+  <si>
+    <t>ASM-1935</t>
+  </si>
+  <si>
+    <t>ASM-1940</t>
+  </si>
+  <si>
+    <t>ASM-1982</t>
+  </si>
+  <si>
+    <t>ASM-1985</t>
+  </si>
+  <si>
+    <t>ASM-1986</t>
+  </si>
+  <si>
+    <t>ASM-2019</t>
+  </si>
+  <si>
+    <t>ASM-2028</t>
+  </si>
+  <si>
+    <t>ASM-2032</t>
+  </si>
+  <si>
+    <t>ASM-2042</t>
+  </si>
+  <si>
+    <t>ASM-2045</t>
+  </si>
+  <si>
+    <t>ASM-2065</t>
+  </si>
+  <si>
+    <t>ASM-2072</t>
+  </si>
+  <si>
+    <t>ASM-2085</t>
+  </si>
+  <si>
+    <t>ASM-2092</t>
+  </si>
+  <si>
+    <t>ASM-2129</t>
+  </si>
+  <si>
+    <t>ASM-2146</t>
+  </si>
+  <si>
+    <t>ASM-2157</t>
+  </si>
+  <si>
+    <t>ASM-2187</t>
+  </si>
+  <si>
+    <t>ASM-2218</t>
+  </si>
+  <si>
+    <t>ASM-2229</t>
+  </si>
+  <si>
+    <t>ASM-2245</t>
+  </si>
+  <si>
+    <t>ASM-2252</t>
+  </si>
+  <si>
+    <t>ASM-2271</t>
+  </si>
+  <si>
+    <t>ASM-2276</t>
+  </si>
+  <si>
+    <t>ASM-2278</t>
+  </si>
+  <si>
+    <t>ASM-2282</t>
+  </si>
+  <si>
+    <t>ASM-2283</t>
+  </si>
+  <si>
+    <t>ASM-2284</t>
+  </si>
+  <si>
+    <t>ASM-2290</t>
+  </si>
+  <si>
+    <t>ASM-2303</t>
+  </si>
+  <si>
+    <t>ASM-2304</t>
+  </si>
+  <si>
+    <t>ASM-2308</t>
+  </si>
+  <si>
+    <t>ASM-2313</t>
+  </si>
+  <si>
+    <t>ASM-2318</t>
+  </si>
+  <si>
+    <t>ASM-2324</t>
+  </si>
+  <si>
+    <t>ASM-2329</t>
+  </si>
+  <si>
+    <t>ASM-2338</t>
+  </si>
+  <si>
+    <t>ASM-2339</t>
+  </si>
+  <si>
+    <t>ASM-2349</t>
+  </si>
+  <si>
+    <t>ASM-2353</t>
+  </si>
+  <si>
+    <t>ASM-2364</t>
+  </si>
+  <si>
+    <t>ASM-2367</t>
+  </si>
+  <si>
+    <t>ASM-2372</t>
+  </si>
+  <si>
+    <t>ASM-2374</t>
+  </si>
+  <si>
+    <t>ASM-2383</t>
+  </si>
+  <si>
+    <t>ASM-2385</t>
+  </si>
+  <si>
+    <t>ASM-2397</t>
+  </si>
+  <si>
+    <t>ASM-2402</t>
+  </si>
+  <si>
+    <t>ASM-2407</t>
+  </si>
+  <si>
+    <t>ASM-2418</t>
+  </si>
+  <si>
+    <t>ASM-2420</t>
+  </si>
+  <si>
+    <t>ASM-2433</t>
+  </si>
+  <si>
+    <t>ASM-2441</t>
+  </si>
+  <si>
+    <t>ASM-2450</t>
+  </si>
+  <si>
+    <t>ASM-2451</t>
+  </si>
+  <si>
+    <t>ASM-2501</t>
+  </si>
+  <si>
+    <t>ASM-2516</t>
+  </si>
+  <si>
+    <t>ASM-2555</t>
+  </si>
+  <si>
+    <t>ASM-2558</t>
+  </si>
+  <si>
+    <t>ASM-2586</t>
+  </si>
+  <si>
+    <t>ASM-2593</t>
+  </si>
+  <si>
+    <t>ASM-2595</t>
+  </si>
+  <si>
+    <t>ASM-2600</t>
+  </si>
+  <si>
+    <t>ASM-2602</t>
+  </si>
+  <si>
+    <t>ASM-2619</t>
+  </si>
+  <si>
+    <t>ASM-2620</t>
+  </si>
+  <si>
+    <t>ASM-2624</t>
+  </si>
+  <si>
+    <t>ASM-2631</t>
+  </si>
+  <si>
+    <t>ASM-2647</t>
+  </si>
+  <si>
+    <t>ASM-2658</t>
+  </si>
+  <si>
+    <t>ASM-2671</t>
+  </si>
+  <si>
+    <t>ASM-2672</t>
+  </si>
+  <si>
+    <t>ASM-2684</t>
+  </si>
+  <si>
+    <t>ASM-2690</t>
+  </si>
+  <si>
+    <t>ASM-2704</t>
+  </si>
+  <si>
+    <t>ASM-2712</t>
+  </si>
+  <si>
+    <t>ASM-2736</t>
+  </si>
+  <si>
+    <t>ASM-2753</t>
+  </si>
+  <si>
+    <t>ASM-2757</t>
+  </si>
+  <si>
+    <t>ASM-2760</t>
+  </si>
+  <si>
+    <t>ASM-2762</t>
+  </si>
+  <si>
+    <t>ASM-2770</t>
+  </si>
+  <si>
+    <t>ASM-2773</t>
+  </si>
+  <si>
+    <t>ASM-2785</t>
+  </si>
+  <si>
+    <t>ASM-2786</t>
+  </si>
+  <si>
+    <t>ASM-2798</t>
+  </si>
+  <si>
+    <t>ASM-2811</t>
+  </si>
+  <si>
+    <t>ASM-2835</t>
+  </si>
+  <si>
+    <t>ASM-2841</t>
+  </si>
+  <si>
+    <t>ASM-2856</t>
+  </si>
+  <si>
+    <t>ASM-2862</t>
+  </si>
+  <si>
+    <t>ASM-2874</t>
+  </si>
+  <si>
+    <t>ASM-2892</t>
+  </si>
+  <si>
+    <t>ASM-2906</t>
+  </si>
+  <si>
+    <t>ASM-2907</t>
+  </si>
+  <si>
+    <t>ASM-2908</t>
+  </si>
+  <si>
+    <t>ASM-2911</t>
+  </si>
+  <si>
+    <t>ASM-2921</t>
+  </si>
+  <si>
+    <t>ASM-2938</t>
+  </si>
+  <si>
+    <t>ASM-2943</t>
+  </si>
+  <si>
+    <t>ASM-2955</t>
+  </si>
+  <si>
+    <t>ASM-2956</t>
+  </si>
+  <si>
+    <t>ASM-2968</t>
+  </si>
+  <si>
+    <t>ASM-2980</t>
+  </si>
+  <si>
+    <t>ASM-2998</t>
+  </si>
+  <si>
+    <t>ASM-3028</t>
   </si>
 </sst>
 </file>
@@ -2741,10 +3356,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G221"/>
+  <dimension ref="A1:J221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A209"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:J209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,9 +3370,11 @@
     <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2768,7 +3385,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>739</v>
       </c>
@@ -2779,7 +3396,7 @@
       <c r="F2" s="31"/>
       <c r="G2" s="32"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>740</v>
       </c>
@@ -2790,7 +3407,7 @@
       <c r="F3" s="34"/>
       <c r="G3" s="35"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2799,7 +3416,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>731</v>
       </c>
@@ -2821,8 +3438,14 @@
       <c r="G5" s="4" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -2842,8 +3465,15 @@
       <c r="G6" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f>LEFT(D6,8)</f>
+        <v>ASM/0138</v>
+      </c>
+      <c r="J6" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -2865,8 +3495,15 @@
       <c r="G7" s="4" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="str">
+        <f t="shared" ref="I7:I70" si="0">LEFT(D7,8)</f>
+        <v>ASM/0149</v>
+      </c>
+      <c r="J7" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -2888,8 +3525,15 @@
       <c r="G8" s="4" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0198</v>
+      </c>
+      <c r="J8" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -2909,8 +3553,15 @@
       <c r="G9" s="4" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0211</v>
+      </c>
+      <c r="J9" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -2928,8 +3579,15 @@
       <c r="G10" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0369</v>
+      </c>
+      <c r="J10" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -2949,8 +3607,15 @@
       <c r="G11" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0404</v>
+      </c>
+      <c r="J11" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -2972,8 +3637,15 @@
       <c r="G12" s="4" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0414</v>
+      </c>
+      <c r="J12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -2995,8 +3667,15 @@
       <c r="G13" s="4" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0425</v>
+      </c>
+      <c r="J13" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -3018,8 +3697,15 @@
       <c r="G14" s="4" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0428</v>
+      </c>
+      <c r="J14" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>10</v>
       </c>
@@ -3041,8 +3727,15 @@
       <c r="G15" s="4" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0429</v>
+      </c>
+      <c r="J15" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>11</v>
       </c>
@@ -3062,8 +3755,15 @@
       <c r="G16" s="4" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0507</v>
+      </c>
+      <c r="J16" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>12</v>
       </c>
@@ -3085,8 +3785,15 @@
       <c r="G17" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0522</v>
+      </c>
+      <c r="J17" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>13</v>
       </c>
@@ -3108,8 +3815,15 @@
       <c r="G18" s="4" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0583</v>
+      </c>
+      <c r="J18" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>14</v>
       </c>
@@ -3131,8 +3845,15 @@
       <c r="G19" s="4" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0664</v>
+      </c>
+      <c r="J19" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>15</v>
       </c>
@@ -3154,8 +3875,15 @@
       <c r="G20" s="4" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0668</v>
+      </c>
+      <c r="J20" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>16</v>
       </c>
@@ -3177,8 +3905,15 @@
       <c r="G21" s="4" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0669</v>
+      </c>
+      <c r="J21" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>17</v>
       </c>
@@ -3200,8 +3935,15 @@
       <c r="G22" s="4" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0675</v>
+      </c>
+      <c r="J22" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>18</v>
       </c>
@@ -3223,8 +3965,15 @@
       <c r="G23" s="4" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0679</v>
+      </c>
+      <c r="J23" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>19</v>
       </c>
@@ -3242,8 +3991,15 @@
       <c r="G24" s="4" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0694</v>
+      </c>
+      <c r="J24" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>20</v>
       </c>
@@ -3265,8 +4021,15 @@
       <c r="G25" s="4" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0696</v>
+      </c>
+      <c r="J25" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>21</v>
       </c>
@@ -3286,8 +4049,15 @@
       <c r="G26" s="4" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0709</v>
+      </c>
+      <c r="J26" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>22</v>
       </c>
@@ -3309,8 +4079,15 @@
       <c r="G27" s="4" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0746</v>
+      </c>
+      <c r="J27" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>23</v>
       </c>
@@ -3332,8 +4109,15 @@
       <c r="G28" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0757</v>
+      </c>
+      <c r="J28" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>24</v>
       </c>
@@ -3355,8 +4139,15 @@
       <c r="G29" s="4" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0819</v>
+      </c>
+      <c r="J29" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>25</v>
       </c>
@@ -3378,8 +4169,15 @@
       <c r="G30" s="4" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0825</v>
+      </c>
+      <c r="J30" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>26</v>
       </c>
@@ -3401,8 +4199,15 @@
       <c r="G31" s="4" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0829</v>
+      </c>
+      <c r="J31" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>27</v>
       </c>
@@ -3424,8 +4229,15 @@
       <c r="G32" s="4" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0850</v>
+      </c>
+      <c r="J32" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>28</v>
       </c>
@@ -3447,8 +4259,15 @@
       <c r="G33" s="4" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0873</v>
+      </c>
+      <c r="J33" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>29</v>
       </c>
@@ -3468,8 +4287,15 @@
       <c r="G34" s="4" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0877</v>
+      </c>
+      <c r="J34" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>30</v>
       </c>
@@ -3491,8 +4317,15 @@
       <c r="G35" s="4" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0882</v>
+      </c>
+      <c r="J35" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>31</v>
       </c>
@@ -3512,8 +4345,15 @@
       <c r="G36" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0904</v>
+      </c>
+      <c r="J36" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>32</v>
       </c>
@@ -3533,8 +4373,15 @@
       <c r="G37" s="4" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0918</v>
+      </c>
+      <c r="J37" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>33</v>
       </c>
@@ -3554,8 +4401,15 @@
       <c r="G38" s="4" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0924</v>
+      </c>
+      <c r="J38" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>34</v>
       </c>
@@ -3575,8 +4429,15 @@
       <c r="G39" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0925</v>
+      </c>
+      <c r="J39" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>35</v>
       </c>
@@ -3596,8 +4457,15 @@
       <c r="G40" s="4" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0959</v>
+      </c>
+      <c r="J40" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>36</v>
       </c>
@@ -3619,8 +4487,15 @@
       <c r="G41" s="4" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0962</v>
+      </c>
+      <c r="J41" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>37</v>
       </c>
@@ -3638,8 +4513,15 @@
       <c r="G42" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0964</v>
+      </c>
+      <c r="J42" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>38</v>
       </c>
@@ -3661,8 +4543,15 @@
       <c r="G43" s="4" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/0992</v>
+      </c>
+      <c r="J43" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>39</v>
       </c>
@@ -3684,8 +4573,15 @@
       <c r="G44" s="4" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1006</v>
+      </c>
+      <c r="J44" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>40</v>
       </c>
@@ -3705,8 +4601,15 @@
       <c r="G45" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1024</v>
+      </c>
+      <c r="J45" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>41</v>
       </c>
@@ -3728,8 +4631,15 @@
       <c r="G46" s="4" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1030</v>
+      </c>
+      <c r="J46" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>42</v>
       </c>
@@ -3749,8 +4659,15 @@
       <c r="G47" s="4" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1082</v>
+      </c>
+      <c r="J47" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43</v>
       </c>
@@ -3772,8 +4689,15 @@
       <c r="G48" s="4" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1108</v>
+      </c>
+      <c r="J48" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>44</v>
       </c>
@@ -3795,8 +4719,15 @@
       <c r="G49" s="4" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1113</v>
+      </c>
+      <c r="J49" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>45</v>
       </c>
@@ -3816,8 +4747,15 @@
       <c r="G50" s="4" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1135</v>
+      </c>
+      <c r="J50" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>46</v>
       </c>
@@ -3839,8 +4777,15 @@
       <c r="G51" s="4" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1148</v>
+      </c>
+      <c r="J51" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>47</v>
       </c>
@@ -3862,8 +4807,15 @@
       <c r="G52" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1160</v>
+      </c>
+      <c r="J52" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>48</v>
       </c>
@@ -3885,8 +4837,15 @@
       <c r="G53" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1183</v>
+      </c>
+      <c r="J53" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>49</v>
       </c>
@@ -3906,8 +4865,15 @@
       <c r="G54" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1185</v>
+      </c>
+      <c r="J54" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>50</v>
       </c>
@@ -3929,8 +4895,15 @@
       <c r="G55" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I55" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1214</v>
+      </c>
+      <c r="J55" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>51</v>
       </c>
@@ -3950,8 +4923,15 @@
       <c r="G56" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I56" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1224</v>
+      </c>
+      <c r="J56" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>52</v>
       </c>
@@ -3973,8 +4953,15 @@
       <c r="G57" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1232</v>
+      </c>
+      <c r="J57" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>53</v>
       </c>
@@ -3992,8 +4979,15 @@
       <c r="G58" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I58" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1240</v>
+      </c>
+      <c r="J58" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>54</v>
       </c>
@@ -4015,8 +5009,15 @@
       <c r="G59" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I59" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1269</v>
+      </c>
+      <c r="J59" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>55</v>
       </c>
@@ -4038,8 +5039,15 @@
       <c r="G60" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I60" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1296</v>
+      </c>
+      <c r="J60" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>56</v>
       </c>
@@ -4061,8 +5069,15 @@
       <c r="G61" s="4" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I61" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1321</v>
+      </c>
+      <c r="J61" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>57</v>
       </c>
@@ -4084,8 +5099,15 @@
       <c r="G62" s="4" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I62" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1363</v>
+      </c>
+      <c r="J62" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>58</v>
       </c>
@@ -4105,8 +5127,15 @@
       <c r="G63" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I63" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1375</v>
+      </c>
+      <c r="J63" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>59</v>
       </c>
@@ -4128,8 +5157,15 @@
       <c r="G64" s="4" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1383</v>
+      </c>
+      <c r="J64" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>60</v>
       </c>
@@ -4151,8 +5187,15 @@
       <c r="G65" s="4" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I65" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1398</v>
+      </c>
+      <c r="J65" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>61</v>
       </c>
@@ -4174,8 +5217,15 @@
       <c r="G66" s="4" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I66" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1403</v>
+      </c>
+      <c r="J66" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>62</v>
       </c>
@@ -4195,8 +5245,15 @@
       <c r="G67" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I67" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1421</v>
+      </c>
+      <c r="J67" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>63</v>
       </c>
@@ -4218,8 +5275,15 @@
       <c r="G68" s="4" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I68" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1467</v>
+      </c>
+      <c r="J68" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>64</v>
       </c>
@@ -4241,8 +5305,15 @@
       <c r="G69" s="4" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I69" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1473</v>
+      </c>
+      <c r="J69" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>65</v>
       </c>
@@ -4264,8 +5335,15 @@
       <c r="G70" s="4" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I70" t="str">
+        <f t="shared" si="0"/>
+        <v>ASM/1501</v>
+      </c>
+      <c r="J70" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>66</v>
       </c>
@@ -4287,8 +5365,15 @@
       <c r="G71" s="4" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I71" t="str">
+        <f t="shared" ref="I71:I134" si="1">LEFT(D71,8)</f>
+        <v>ASM/1522</v>
+      </c>
+      <c r="J71" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>67</v>
       </c>
@@ -4310,8 +5395,15 @@
       <c r="G72" s="4" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I72" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1526</v>
+      </c>
+      <c r="J72" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>68</v>
       </c>
@@ -4333,8 +5425,15 @@
       <c r="G73" s="4" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I73" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1535</v>
+      </c>
+      <c r="J73" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>69</v>
       </c>
@@ -4356,8 +5455,15 @@
       <c r="G74" s="4" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I74" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1538</v>
+      </c>
+      <c r="J74" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>70</v>
       </c>
@@ -4379,8 +5485,15 @@
       <c r="G75" s="4" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I75" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1540</v>
+      </c>
+      <c r="J75" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>71</v>
       </c>
@@ -4400,8 +5513,15 @@
       <c r="G76" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I76" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1548</v>
+      </c>
+      <c r="J76" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>72</v>
       </c>
@@ -4421,8 +5541,15 @@
       <c r="G77" s="4" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I77" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1572</v>
+      </c>
+      <c r="J77" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>73</v>
       </c>
@@ -4442,8 +5569,15 @@
       <c r="G78" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I78" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1599</v>
+      </c>
+      <c r="J78" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>74</v>
       </c>
@@ -4465,8 +5599,15 @@
       <c r="G79" s="4" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I79" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1602</v>
+      </c>
+      <c r="J79" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>75</v>
       </c>
@@ -4488,8 +5629,15 @@
       <c r="G80" s="4" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I80" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1603</v>
+      </c>
+      <c r="J80" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>76</v>
       </c>
@@ -4511,8 +5659,15 @@
       <c r="G81" s="4" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I81" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1604</v>
+      </c>
+      <c r="J81" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>77</v>
       </c>
@@ -4534,8 +5689,15 @@
       <c r="G82" s="4" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I82" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1606</v>
+      </c>
+      <c r="J82" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>78</v>
       </c>
@@ -4557,8 +5719,15 @@
       <c r="G83" s="4" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I83" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1631</v>
+      </c>
+      <c r="J83" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>79</v>
       </c>
@@ -4578,8 +5747,15 @@
       <c r="G84" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I84" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1639</v>
+      </c>
+      <c r="J84" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>80</v>
       </c>
@@ -4601,8 +5777,15 @@
       <c r="G85" s="4" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I85" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1648</v>
+      </c>
+      <c r="J85" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>81</v>
       </c>
@@ -4620,8 +5803,15 @@
       <c r="G86" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I86" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1658</v>
+      </c>
+      <c r="J86" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>82</v>
       </c>
@@ -4641,8 +5831,15 @@
       <c r="G87" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I87" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1666</v>
+      </c>
+      <c r="J87" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>83</v>
       </c>
@@ -4664,8 +5861,15 @@
       <c r="G88" s="4" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I88" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1689</v>
+      </c>
+      <c r="J88" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>84</v>
       </c>
@@ -4685,8 +5889,15 @@
       <c r="G89" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I89" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1707</v>
+      </c>
+      <c r="J89" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>85</v>
       </c>
@@ -4708,8 +5919,15 @@
       <c r="G90" s="4" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I90" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1731</v>
+      </c>
+      <c r="J90" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>86</v>
       </c>
@@ -4731,8 +5949,15 @@
       <c r="G91" s="4" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I91" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1732</v>
+      </c>
+      <c r="J91" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>87</v>
       </c>
@@ -4750,8 +5975,15 @@
       <c r="G92" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I92" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1759</v>
+      </c>
+      <c r="J92" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>88</v>
       </c>
@@ -4771,8 +6003,15 @@
       <c r="G93" s="4" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I93" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1768</v>
+      </c>
+      <c r="J93" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>89</v>
       </c>
@@ -4794,8 +6033,15 @@
       <c r="G94" s="4" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I94" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1772</v>
+      </c>
+      <c r="J94" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>90</v>
       </c>
@@ -4817,8 +6063,15 @@
       <c r="G95" s="4" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I95" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1775</v>
+      </c>
+      <c r="J95" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>91</v>
       </c>
@@ -4838,8 +6091,15 @@
       <c r="G96" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I96" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1790</v>
+      </c>
+      <c r="J96" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>92</v>
       </c>
@@ -4861,8 +6121,15 @@
       <c r="G97" s="4" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I97" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1860</v>
+      </c>
+      <c r="J97" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>93</v>
       </c>
@@ -4882,8 +6149,15 @@
       <c r="G98" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I98" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1872</v>
+      </c>
+      <c r="J98" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>94</v>
       </c>
@@ -4903,8 +6177,15 @@
       <c r="G99" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I99" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1906</v>
+      </c>
+      <c r="J99" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>95</v>
       </c>
@@ -4926,8 +6207,15 @@
       <c r="G100" s="4" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I100" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1908</v>
+      </c>
+      <c r="J100" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>96</v>
       </c>
@@ -4949,8 +6237,15 @@
       <c r="G101" s="4" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I101" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1916</v>
+      </c>
+      <c r="J101" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>97</v>
       </c>
@@ -4972,8 +6267,15 @@
       <c r="G102" s="4" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I102" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1918</v>
+      </c>
+      <c r="J102" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>98</v>
       </c>
@@ -4993,8 +6295,15 @@
       <c r="G103" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I103" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1927</v>
+      </c>
+      <c r="J103" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>99</v>
       </c>
@@ -5014,8 +6323,15 @@
       <c r="G104" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I104" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1935</v>
+      </c>
+      <c r="J104" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>100</v>
       </c>
@@ -5037,8 +6353,15 @@
       <c r="G105" s="4" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I105" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1940</v>
+      </c>
+      <c r="J105" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>101</v>
       </c>
@@ -5060,8 +6383,15 @@
       <c r="G106" s="4" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I106" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1982</v>
+      </c>
+      <c r="J106" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>102</v>
       </c>
@@ -5083,8 +6413,15 @@
       <c r="G107" s="4" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I107" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1985</v>
+      </c>
+      <c r="J107" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>103</v>
       </c>
@@ -5104,8 +6441,15 @@
       <c r="G108" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I108" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/1986</v>
+      </c>
+      <c r="J108" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>104</v>
       </c>
@@ -5127,8 +6471,15 @@
       <c r="G109" s="4" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I109" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2019</v>
+      </c>
+      <c r="J109" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>105</v>
       </c>
@@ -5148,8 +6499,15 @@
       <c r="G110" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I110" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2028</v>
+      </c>
+      <c r="J110" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>106</v>
       </c>
@@ -5171,8 +6529,15 @@
       <c r="G111" s="4" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I111" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2032</v>
+      </c>
+      <c r="J111" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>107</v>
       </c>
@@ -5194,8 +6559,15 @@
       <c r="G112" s="4" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I112" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2042</v>
+      </c>
+      <c r="J112" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>108</v>
       </c>
@@ -5215,8 +6587,15 @@
       <c r="G113" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I113" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2045</v>
+      </c>
+      <c r="J113" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>109</v>
       </c>
@@ -5236,8 +6615,15 @@
       <c r="G114" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I114" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2065</v>
+      </c>
+      <c r="J114" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>110</v>
       </c>
@@ -5259,8 +6645,15 @@
       <c r="G115" s="4" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I115" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2072</v>
+      </c>
+      <c r="J115" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>111</v>
       </c>
@@ -5282,8 +6675,15 @@
       <c r="G116" s="4" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I116" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2085</v>
+      </c>
+      <c r="J116" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>112</v>
       </c>
@@ -5303,8 +6703,15 @@
       <c r="G117" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I117" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2092</v>
+      </c>
+      <c r="J117" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>113</v>
       </c>
@@ -5326,8 +6733,15 @@
       <c r="G118" s="4" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I118" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2129</v>
+      </c>
+      <c r="J118" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>114</v>
       </c>
@@ -5349,8 +6763,15 @@
       <c r="G119" s="4" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I119" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2146</v>
+      </c>
+      <c r="J119" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>115</v>
       </c>
@@ -5372,8 +6793,15 @@
       <c r="G120" s="4" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I120" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2157</v>
+      </c>
+      <c r="J120" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>116</v>
       </c>
@@ -5393,8 +6821,15 @@
       <c r="G121" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I121" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2187</v>
+      </c>
+      <c r="J121" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>117</v>
       </c>
@@ -5416,8 +6851,15 @@
       <c r="G122" s="4" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I122" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2218</v>
+      </c>
+      <c r="J122" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>118</v>
       </c>
@@ -5439,8 +6881,15 @@
       <c r="G123" s="4" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I123" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2229</v>
+      </c>
+      <c r="J123" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>119</v>
       </c>
@@ -5460,8 +6909,15 @@
       <c r="G124" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I124" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2245</v>
+      </c>
+      <c r="J124" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>120</v>
       </c>
@@ -5481,8 +6937,15 @@
       <c r="G125" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I125" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2252</v>
+      </c>
+      <c r="J125" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>121</v>
       </c>
@@ -5502,8 +6965,15 @@
       <c r="G126" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I126" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2271</v>
+      </c>
+      <c r="J126" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>122</v>
       </c>
@@ -5525,8 +6995,15 @@
       <c r="G127" s="4" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I127" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2276</v>
+      </c>
+      <c r="J127" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>123</v>
       </c>
@@ -5546,8 +7023,15 @@
       <c r="G128" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I128" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2278</v>
+      </c>
+      <c r="J128" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>124</v>
       </c>
@@ -5567,8 +7051,15 @@
       <c r="G129" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I129" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2282</v>
+      </c>
+      <c r="J129" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>125</v>
       </c>
@@ -5588,8 +7079,15 @@
       <c r="G130" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I130" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2283</v>
+      </c>
+      <c r="J130" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>126</v>
       </c>
@@ -5609,8 +7107,15 @@
       <c r="G131" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I131" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2284</v>
+      </c>
+      <c r="J131" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>127</v>
       </c>
@@ -5630,8 +7135,15 @@
       <c r="G132" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I132" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2290</v>
+      </c>
+      <c r="J132" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>128</v>
       </c>
@@ -5653,8 +7165,15 @@
       <c r="G133" s="4" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I133" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2303</v>
+      </c>
+      <c r="J133" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>129</v>
       </c>
@@ -5676,8 +7195,15 @@
       <c r="G134" s="4" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I134" t="str">
+        <f t="shared" si="1"/>
+        <v>ASM/2304</v>
+      </c>
+      <c r="J134" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>130</v>
       </c>
@@ -5697,8 +7223,15 @@
       <c r="G135" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I135" t="str">
+        <f t="shared" ref="I135:I198" si="2">LEFT(D135,8)</f>
+        <v>ASM/2308</v>
+      </c>
+      <c r="J135" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>131</v>
       </c>
@@ -5718,8 +7251,15 @@
       <c r="G136" s="4" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I136" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2313</v>
+      </c>
+      <c r="J136" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>132</v>
       </c>
@@ -5741,8 +7281,15 @@
       <c r="G137" s="4" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I137" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2318</v>
+      </c>
+      <c r="J137" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>133</v>
       </c>
@@ -5762,8 +7309,15 @@
       <c r="G138" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I138" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2324</v>
+      </c>
+      <c r="J138" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>134</v>
       </c>
@@ -5783,8 +7337,15 @@
       <c r="G139" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I139" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2329</v>
+      </c>
+      <c r="J139" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>135</v>
       </c>
@@ -5806,8 +7367,15 @@
       <c r="G140" s="4" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I140" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2338</v>
+      </c>
+      <c r="J140" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>136</v>
       </c>
@@ -5829,8 +7397,15 @@
       <c r="G141" s="4" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I141" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2339</v>
+      </c>
+      <c r="J141" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>137</v>
       </c>
@@ -5850,8 +7425,15 @@
       <c r="G142" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I142" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2349</v>
+      </c>
+      <c r="J142" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>138</v>
       </c>
@@ -5871,8 +7453,15 @@
       <c r="G143" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I143" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2353</v>
+      </c>
+      <c r="J143" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>139</v>
       </c>
@@ -5892,8 +7481,15 @@
       <c r="G144" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I144" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2364</v>
+      </c>
+      <c r="J144" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>140</v>
       </c>
@@ -5915,8 +7511,15 @@
       <c r="G145" s="4" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I145" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2367</v>
+      </c>
+      <c r="J145" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>141</v>
       </c>
@@ -5938,8 +7541,15 @@
       <c r="G146" s="4" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I146" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2372</v>
+      </c>
+      <c r="J146" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>142</v>
       </c>
@@ -5961,8 +7571,15 @@
       <c r="G147" s="4" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I147" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2374</v>
+      </c>
+      <c r="J147" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>143</v>
       </c>
@@ -5984,8 +7601,15 @@
       <c r="G148" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I148" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2383</v>
+      </c>
+      <c r="J148" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>144</v>
       </c>
@@ -6005,8 +7629,15 @@
       <c r="G149" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I149" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2385</v>
+      </c>
+      <c r="J149" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>145</v>
       </c>
@@ -6028,8 +7659,15 @@
       <c r="G150" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I150" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2397</v>
+      </c>
+      <c r="J150" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>146</v>
       </c>
@@ -6051,8 +7689,15 @@
       <c r="G151" s="4" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I151" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2402</v>
+      </c>
+      <c r="J151" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>147</v>
       </c>
@@ -6072,8 +7717,15 @@
       <c r="G152" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I152" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2407</v>
+      </c>
+      <c r="J152" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>148</v>
       </c>
@@ -6093,8 +7745,15 @@
       <c r="G153" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I153" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2418</v>
+      </c>
+      <c r="J153" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>149</v>
       </c>
@@ -6114,8 +7773,15 @@
       <c r="G154" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I154" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2420</v>
+      </c>
+      <c r="J154" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>150</v>
       </c>
@@ -6135,8 +7801,15 @@
       <c r="G155" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I155" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2433</v>
+      </c>
+      <c r="J155" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>151</v>
       </c>
@@ -6156,8 +7829,15 @@
       <c r="G156" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I156" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2441</v>
+      </c>
+      <c r="J156" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>152</v>
       </c>
@@ -6179,8 +7859,15 @@
       <c r="G157" s="4" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I157" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2450</v>
+      </c>
+      <c r="J157" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>153</v>
       </c>
@@ -6200,8 +7887,15 @@
       <c r="G158" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I158" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2451</v>
+      </c>
+      <c r="J158" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>154</v>
       </c>
@@ -6221,8 +7915,15 @@
       <c r="G159" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I159" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2501</v>
+      </c>
+      <c r="J159" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>155</v>
       </c>
@@ -6244,8 +7945,15 @@
       <c r="G160" s="4" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I160" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2516</v>
+      </c>
+      <c r="J160" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>156</v>
       </c>
@@ -6267,8 +7975,15 @@
       <c r="G161" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I161" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2555</v>
+      </c>
+      <c r="J161" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>157</v>
       </c>
@@ -6288,8 +8003,15 @@
       <c r="G162" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I162" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2558</v>
+      </c>
+      <c r="J162" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>158</v>
       </c>
@@ -6309,8 +8031,15 @@
       <c r="G163" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I163" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2586</v>
+      </c>
+      <c r="J163" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>159</v>
       </c>
@@ -6332,8 +8061,15 @@
       <c r="G164" s="4" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I164" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2593</v>
+      </c>
+      <c r="J164" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>160</v>
       </c>
@@ -6353,8 +8089,15 @@
       <c r="G165" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I165" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2595</v>
+      </c>
+      <c r="J165" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>161</v>
       </c>
@@ -6374,8 +8117,15 @@
       <c r="G166" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I166" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2600</v>
+      </c>
+      <c r="J166" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>162</v>
       </c>
@@ -6395,8 +8145,15 @@
       <c r="G167" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I167" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2602</v>
+      </c>
+      <c r="J167" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>163</v>
       </c>
@@ -6418,8 +8175,15 @@
       <c r="G168" s="4" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I168" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2619</v>
+      </c>
+      <c r="J168" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>164</v>
       </c>
@@ -6441,8 +8205,15 @@
       <c r="G169" s="4" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I169" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2620</v>
+      </c>
+      <c r="J169" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>165</v>
       </c>
@@ -6462,8 +8233,15 @@
       <c r="G170" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I170" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2624</v>
+      </c>
+      <c r="J170" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>166</v>
       </c>
@@ -6483,8 +8261,15 @@
       <c r="G171" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I171" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2631</v>
+      </c>
+      <c r="J171" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>167</v>
       </c>
@@ -6506,8 +8291,15 @@
       <c r="G172" s="4" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I172" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2647</v>
+      </c>
+      <c r="J172" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>168</v>
       </c>
@@ -6527,8 +8319,15 @@
       <c r="G173" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I173" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2658</v>
+      </c>
+      <c r="J173" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>169</v>
       </c>
@@ -6548,8 +8347,15 @@
       <c r="G174" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I174" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2671</v>
+      </c>
+      <c r="J174" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>170</v>
       </c>
@@ -6571,8 +8377,15 @@
       <c r="G175" s="4" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I175" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2672</v>
+      </c>
+      <c r="J175" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>171</v>
       </c>
@@ -6594,8 +8407,15 @@
       <c r="G176" s="4" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I176" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2684</v>
+      </c>
+      <c r="J176" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>172</v>
       </c>
@@ -6615,8 +8435,15 @@
       <c r="G177" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I177" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2690</v>
+      </c>
+      <c r="J177" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>173</v>
       </c>
@@ -6636,8 +8463,15 @@
       <c r="G178" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I178" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2704</v>
+      </c>
+      <c r="J178" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>174</v>
       </c>
@@ -6659,8 +8493,15 @@
       <c r="G179" s="4" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I179" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2712</v>
+      </c>
+      <c r="J179" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>175</v>
       </c>
@@ -6680,8 +8521,15 @@
       <c r="G180" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I180" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2736</v>
+      </c>
+      <c r="J180" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>176</v>
       </c>
@@ -6701,8 +8549,15 @@
       <c r="G181" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I181" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2753</v>
+      </c>
+      <c r="J181" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>177</v>
       </c>
@@ -6722,8 +8577,15 @@
       <c r="G182" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I182" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2757</v>
+      </c>
+      <c r="J182" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>178</v>
       </c>
@@ -6743,8 +8605,15 @@
       <c r="G183" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I183" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2760</v>
+      </c>
+      <c r="J183" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>179</v>
       </c>
@@ -6766,8 +8635,15 @@
       <c r="G184" s="4" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I184" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2762</v>
+      </c>
+      <c r="J184" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>180</v>
       </c>
@@ -6789,8 +8665,15 @@
       <c r="G185" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I185" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2770</v>
+      </c>
+      <c r="J185" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>181</v>
       </c>
@@ -6812,8 +8695,15 @@
       <c r="G186" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I186" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2773</v>
+      </c>
+      <c r="J186" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>182</v>
       </c>
@@ -6835,8 +8725,15 @@
       <c r="G187" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I187" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2785</v>
+      </c>
+      <c r="J187" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>183</v>
       </c>
@@ -6858,8 +8755,15 @@
       <c r="G188" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I188" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2786</v>
+      </c>
+      <c r="J188" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>184</v>
       </c>
@@ -6881,8 +8785,15 @@
       <c r="G189" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I189" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2798</v>
+      </c>
+      <c r="J189" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>185</v>
       </c>
@@ -6904,8 +8815,15 @@
       <c r="G190" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I190" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2811</v>
+      </c>
+      <c r="J190" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>186</v>
       </c>
@@ -6927,8 +8845,15 @@
       <c r="G191" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I191" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2835</v>
+      </c>
+      <c r="J191" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>187</v>
       </c>
@@ -6950,8 +8875,15 @@
       <c r="G192" s="4" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I192" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2841</v>
+      </c>
+      <c r="J192" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>188</v>
       </c>
@@ -6973,8 +8905,15 @@
       <c r="G193" s="4" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I193" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2856</v>
+      </c>
+      <c r="J193" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>189</v>
       </c>
@@ -6996,8 +8935,15 @@
       <c r="G194" s="4" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I194" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2862</v>
+      </c>
+      <c r="J194" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>190</v>
       </c>
@@ -7019,8 +8965,15 @@
       <c r="G195" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I195" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2874</v>
+      </c>
+      <c r="J195" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>191</v>
       </c>
@@ -7042,8 +8995,15 @@
       <c r="G196" s="4" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I196" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2892</v>
+      </c>
+      <c r="J196" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>192</v>
       </c>
@@ -7065,8 +9025,15 @@
       <c r="G197" s="4" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I197" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2906</v>
+      </c>
+      <c r="J197" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>193</v>
       </c>
@@ -7088,8 +9055,15 @@
       <c r="G198" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I198" t="str">
+        <f t="shared" si="2"/>
+        <v>ASM/2907</v>
+      </c>
+      <c r="J198" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>194</v>
       </c>
@@ -7111,8 +9085,15 @@
       <c r="G199" s="4" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I199" t="str">
+        <f t="shared" ref="I199:I210" si="3">LEFT(D199,8)</f>
+        <v>ASM/2908</v>
+      </c>
+      <c r="J199" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>195</v>
       </c>
@@ -7134,8 +9115,15 @@
       <c r="G200" s="4" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I200" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2911</v>
+      </c>
+      <c r="J200" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>196</v>
       </c>
@@ -7157,8 +9145,15 @@
       <c r="G201" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I201" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2921</v>
+      </c>
+      <c r="J201" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>197</v>
       </c>
@@ -7180,8 +9175,15 @@
       <c r="G202" s="4" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I202" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2938</v>
+      </c>
+      <c r="J202" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>198</v>
       </c>
@@ -7203,8 +9205,15 @@
       <c r="G203" s="4" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I203" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2943</v>
+      </c>
+      <c r="J203" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>199</v>
       </c>
@@ -7226,8 +9235,15 @@
       <c r="G204" s="4" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I204" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2955</v>
+      </c>
+      <c r="J204" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>200</v>
       </c>
@@ -7249,8 +9265,15 @@
       <c r="G205" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I205" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2956</v>
+      </c>
+      <c r="J205" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>201</v>
       </c>
@@ -7272,8 +9295,15 @@
       <c r="G206" s="4" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I206" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2968</v>
+      </c>
+      <c r="J206" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>202</v>
       </c>
@@ -7295,8 +9325,15 @@
       <c r="G207" s="4" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I207" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2980</v>
+      </c>
+      <c r="J207" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>203</v>
       </c>
@@ -7318,8 +9355,15 @@
       <c r="G208" s="4" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I208" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/2998</v>
+      </c>
+      <c r="J208" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>204</v>
       </c>
@@ -7341,8 +9385,15 @@
       <c r="G209" s="4" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I209" t="str">
+        <f t="shared" si="3"/>
+        <v>ASM/3028</v>
+      </c>
+      <c r="J209" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="15"/>
       <c r="B210" s="16"/>
       <c r="C210" s="16"/>
@@ -7353,7 +9404,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="20"/>
       <c r="B211" s="21"/>
       <c r="C211" s="21"/>
@@ -7362,7 +9413,7 @@
       <c r="F211" s="23"/>
       <c r="G211" s="24"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="20"/>
       <c r="B212" s="21"/>
       <c r="C212" s="21"/>
@@ -7371,7 +9422,7 @@
       <c r="F212" s="23"/>
       <c r="G212" s="24"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="20"/>
       <c r="B213" s="21"/>
       <c r="C213" s="21"/>
@@ -7380,7 +9431,7 @@
       <c r="F213" s="23"/>
       <c r="G213" s="24"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="20"/>
       <c r="B214" s="21"/>
       <c r="C214" s="21"/>
@@ -7389,7 +9440,7 @@
       <c r="F214" s="23"/>
       <c r="G214" s="24"/>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="20"/>
       <c r="B215" s="21"/>
       <c r="C215" s="21"/>
@@ -7398,7 +9449,7 @@
       <c r="F215" s="23"/>
       <c r="G215" s="24"/>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="20"/>
       <c r="B216" s="21"/>
       <c r="C216" s="21"/>
@@ -7407,7 +9458,7 @@
       <c r="F216" s="23"/>
       <c r="G216" s="24"/>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="20"/>
       <c r="B217" s="21"/>
       <c r="C217" s="21"/>
@@ -7416,7 +9467,7 @@
       <c r="F217" s="23"/>
       <c r="G217" s="24"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="20"/>
       <c r="B218" s="21"/>
       <c r="C218" s="21"/>
@@ -7425,7 +9476,7 @@
       <c r="F218" s="23"/>
       <c r="G218" s="24"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="20"/>
       <c r="B219" s="21"/>
       <c r="C219" s="21"/>
@@ -7434,7 +9485,7 @@
       <c r="F219" s="23"/>
       <c r="G219" s="24"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="20"/>
       <c r="B220" s="21"/>
       <c r="C220" s="21"/>
@@ -7443,7 +9494,7 @@
       <c r="F220" s="23"/>
       <c r="G220" s="24"/>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="25"/>
       <c r="B221" s="26"/>
       <c r="C221" s="26"/>

</xml_diff>